<commit_message>
brython was a bad idea...
</commit_message>
<xml_diff>
--- a/static/xlsx/CabaretTix.xlsx
+++ b/static/xlsx/CabaretTix.xlsx
@@ -607,7 +607,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -626,9 +626,6 @@
       <sz val="18.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="18.0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -671,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -713,20 +710,6 @@
     </xf>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -949,14 +932,13 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" hidden="1" min="1" max="1" width="21.57"/>
+    <col customWidth="1" min="1" max="1" width="21.57"/>
     <col customWidth="1" min="2" max="2" width="43.29"/>
-    <col customWidth="1" min="3" max="10" width="21.57"/>
-    <col customWidth="1" hidden="1" min="11" max="12" width="21.57"/>
+    <col customWidth="1" min="3" max="12" width="21.57"/>
     <col customWidth="1" min="13" max="13" width="11.14"/>
     <col customWidth="1" min="14" max="14" width="17.71"/>
     <col customWidth="1" min="15" max="15" width="69.86"/>
-    <col customWidth="1" hidden="1" min="16" max="17" width="21.57"/>
+    <col customWidth="1" min="16" max="17" width="21.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3237,118 +3219,118 @@
       <c r="A57" s="15">
         <v>44494.33839576389</v>
       </c>
-      <c r="B57" s="19" t="s">
+      <c r="B57" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C57" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D57" s="20"/>
-      <c r="E57" s="19">
+      <c r="D57" s="10"/>
+      <c r="E57" s="9">
         <v>6.1988905E9</v>
       </c>
-      <c r="F57" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="G57" s="19">
+      <c r="F57" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="G57" s="9">
         <v>7.0</v>
       </c>
-      <c r="H57" s="19">
+      <c r="H57" s="9">
         <v>5.0</v>
       </c>
-      <c r="I57" s="19">
-        <v>12.0</v>
-      </c>
-      <c r="J57" s="19">
-        <v>120.0</v>
-      </c>
-      <c r="K57" s="19" t="s">
+      <c r="I57" s="9">
+        <v>12.0</v>
+      </c>
+      <c r="J57" s="9">
+        <v>120.0</v>
+      </c>
+      <c r="K57" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="L57" s="19" t="s">
+      <c r="L57" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="M57" s="20"/>
-      <c r="N57" s="20"/>
-      <c r="O57" s="20"/>
+      <c r="M57" s="10"/>
+      <c r="N57" s="10"/>
+      <c r="O57" s="10"/>
     </row>
     <row r="58">
       <c r="A58" s="15">
         <v>44494.424870462964</v>
       </c>
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="C58" s="21" t="s">
+      <c r="C58" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="21">
+      <c r="D58" s="17"/>
+      <c r="E58" s="16">
         <v>5.132272619E9</v>
       </c>
-      <c r="F58" s="21">
+      <c r="F58" s="16">
         <v>4.0</v>
       </c>
-      <c r="G58" s="21">
+      <c r="G58" s="16">
         <v>4.0</v>
       </c>
-      <c r="H58" s="21">
+      <c r="H58" s="16">
         <v>4.0</v>
       </c>
-      <c r="I58" s="21">
-        <v>12.0</v>
-      </c>
-      <c r="J58" s="23">
-        <v>120.0</v>
-      </c>
-      <c r="K58" s="21" t="s">
+      <c r="I58" s="16">
+        <v>12.0</v>
+      </c>
+      <c r="J58" s="18">
+        <v>120.0</v>
+      </c>
+      <c r="K58" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="L58" s="21" t="s">
+      <c r="L58" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="M58" s="22"/>
-      <c r="N58" s="22"/>
-      <c r="O58" s="22"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="17"/>
     </row>
     <row r="59">
       <c r="A59" s="15">
         <v>44494.439696319445</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="C59" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="D59" s="20"/>
-      <c r="E59" s="19">
+      <c r="D59" s="10"/>
+      <c r="E59" s="9">
         <v>8.586637633E9</v>
       </c>
-      <c r="F59" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="G59" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="H59" s="19">
-        <v>12.0</v>
-      </c>
-      <c r="I59" s="19">
-        <v>12.0</v>
-      </c>
-      <c r="J59" s="24">
-        <v>120.0</v>
-      </c>
-      <c r="K59" s="19" t="s">
+      <c r="F59" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="G59" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="H59" s="9">
+        <v>12.0</v>
+      </c>
+      <c r="I59" s="9">
+        <v>12.0</v>
+      </c>
+      <c r="J59" s="11">
+        <v>120.0</v>
+      </c>
+      <c r="K59" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L59" s="19" t="s">
+      <c r="L59" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="M59" s="20"/>
-      <c r="N59" s="20"/>
-      <c r="O59" s="20"/>
+      <c r="M59" s="10"/>
+      <c r="N59" s="10"/>
+      <c r="O59" s="10"/>
     </row>
     <row r="60" ht="24.75" customHeight="1">
       <c r="A60" s="12"/>
@@ -3729,9 +3711,18 @@
       <c r="C79" s="10"/>
       <c r="D79" s="10"/>
       <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="10"/>
-      <c r="H79" s="10"/>
+      <c r="F79" s="10">
+        <f t="shared" ref="F79:H79" si="2">375-F76</f>
+        <v>166</v>
+      </c>
+      <c r="G79" s="10">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="H79" s="10">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
       <c r="I79" s="10"/>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>

</xml_diff>